<commit_message>
Adição do codigo e biblioteca pywin32
</commit_message>
<xml_diff>
--- a/Mapeamento/mapeamento.xlsx
+++ b/Mapeamento/mapeamento.xlsx
@@ -435,7 +435,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,19 +485,19 @@
     </row>
     <row r="2">
       <c r="A2" s="3" t="n">
-        <v>150002006</v>
+        <v>150001001</v>
       </c>
       <c r="B2" s="4" t="inlineStr">
         <is>
-          <t>FITA BORDA PS 34/0,45MM - OFF WHITE FOSC</t>
+          <t xml:space="preserve">FITA BORDA PAPEL 18MM PARDO - 180G - NEUTRO  </t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
-        <v>13480</v>
+        <v>3543</v>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
-          <t>R3E</t>
+          <t>R3D</t>
         </is>
       </c>
       <c r="E2" s="2" t="inlineStr">
@@ -513,80 +513,80 @@
     </row>
     <row r="3">
       <c r="A3" s="3" t="n">
-        <v>160006007</v>
+        <v>150001004</v>
       </c>
       <c r="B3" s="4" t="inlineStr">
         <is>
-          <t>PARAFUSO 4,0X16 CABECA CHATA PHS BICROMA</t>
+          <t xml:space="preserve">FITA BORDA PAPEL 18 MM - 210G - JEQUITIBA    </t>
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>40000</v>
+        <v>7070</v>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t>R3E</t>
+          <t>R3D</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>S3</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="F3" s="2" t="inlineStr">
         <is>
-          <t>E1</t>
+          <t>D0</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="n">
-        <v>160006053</v>
+        <v>150001005</v>
       </c>
       <c r="B4" s="4" t="inlineStr">
         <is>
-          <t>PARAFUSO ESTRUTURAL 7X40 CABECA CHATA RO</t>
+          <t>FITA BORDA PAPEL 28 MM - 240G - OFF WHITE FOS</t>
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>28000</v>
+        <v>2023</v>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>R3E</t>
+          <t>R3D</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">
         <is>
-          <t>S3</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="F4" s="2" t="inlineStr">
         <is>
-          <t>E0</t>
+          <t>D1</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="n">
-        <v>160006008</v>
+        <v>150001004</v>
       </c>
       <c r="B5" s="4" t="inlineStr">
         <is>
-          <t>PARAFUSO 4,5X25 CABECA CHATA PHS BICROMA</t>
+          <t xml:space="preserve">FITA BORDA PAPEL 18 MM - 210G - AMENDOA      </t>
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>250000</v>
+        <v>21320</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>R3E</t>
+          <t>R3D</t>
         </is>
       </c>
       <c r="E5" s="2" t="inlineStr">
         <is>
-          <t>S4</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="F5" s="2" t="inlineStr">
@@ -597,55 +597,895 @@
     </row>
     <row r="6">
       <c r="A6" s="3" t="n">
-        <v>160006006</v>
+        <v>150001004</v>
       </c>
       <c r="B6" s="4" t="inlineStr">
         <is>
-          <t>PARAFUSO 3,5X40 CABECA CHATA PHS BICROMA</t>
+          <t xml:space="preserve">FITA BORDA PAPEL 18 MM - 210G - OFF WHITE    </t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>60000</v>
+        <v>2665</v>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>R3E</t>
+          <t>R3D</t>
         </is>
       </c>
       <c r="E6" s="2" t="inlineStr">
         <is>
-          <t>S5</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="F6" s="2" t="inlineStr">
         <is>
-          <t>E0</t>
+          <t>E1</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="n">
+        <v>150001005</v>
+      </c>
+      <c r="B7" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FITA BORDA PAPEL 28 MM - 240G - NATURE       </t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>2640</v>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>R3D</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="n">
+        <v>150002001</v>
+      </c>
+      <c r="B8" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FITA BORDA PS 19/0,45MM - GRIS FOSCO         </t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>4515</v>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>D0</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="n">
+        <v>150001004</v>
+      </c>
+      <c r="B9" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FITA BORDA PAPEL 18 MM - 210G - CARVALHO     </t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>15640</v>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>R3D</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="n">
+        <v>150001004</v>
+      </c>
+      <c r="B10" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FITA BORDA PAPEL 18 MM - 210G - FREIJO       </t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>10320</v>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>R4D</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="n">
+        <v>150001004</v>
+      </c>
+      <c r="B11" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FITA BORDA PAPEL 18 MM - 210G - NATURE       </t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>27980</v>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>R3D</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F11" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="n">
+        <v>150002006</v>
+      </c>
+      <c r="B12" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FITA BORDA PS 34/0,45MM - OFF WHITE FOSCO    </t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>2410</v>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F12" s="2" t="inlineStr">
+        <is>
+          <t>E2</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="n">
+        <v>150002002</v>
+      </c>
+      <c r="B13" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FITA BORDA PS 29X0,45 MM - GRIS FOSCO        </t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n">
+        <v>1552</v>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>R4D</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="inlineStr">
+        <is>
+          <t>S1</t>
+        </is>
+      </c>
+      <c r="F13" s="2" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="n">
+        <v>160002006</v>
+      </c>
+      <c r="B14" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BUCHA 8MM (PAREDE) - NEUTRO                  </t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="F14" s="2" t="inlineStr">
+        <is>
+          <t>D0</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="n">
+        <v>160006015</v>
+      </c>
+      <c r="B15" s="4" t="inlineStr">
+        <is>
+          <t>PARAFUSO 6,0X75 CABECA CHATA PHS BICROMATIZAD</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n">
+        <v>5000</v>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="F15" s="2" t="inlineStr">
+        <is>
+          <t>E0</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="n">
+        <v>150001003</v>
+      </c>
+      <c r="B16" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FITA BORDA PAPEL 40 MM PARDO - 180G - NEUTRO </t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n">
+        <v>1805</v>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>R3D</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="inlineStr">
+        <is>
+          <t>S2</t>
+        </is>
+      </c>
+      <c r="F16" s="2" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="n">
+        <v>160006053</v>
+      </c>
+      <c r="B17" s="4" t="inlineStr">
+        <is>
+          <t>PARAFUSO ESTRUTURAL 7X40 CABECA CHATA ROSCA F</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="F17" s="2" t="inlineStr">
+        <is>
+          <t>E0</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="n">
+        <v>150002007</v>
+      </c>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FITA BORDA PS 22/045MM - OFF WHITE FOSCO     </t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>1500</v>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>R3D</t>
+        </is>
+      </c>
+      <c r="E18" s="2" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="F18" s="2" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="n">
+        <v>160006018</v>
+      </c>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PARAFUSO 4,5X22 CABECA CHATA - ZINCADO       </t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E19" s="2" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="F19" s="2" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="n">
+        <v>160006011</v>
+      </c>
+      <c r="B20" s="4" t="inlineStr">
+        <is>
+          <t>PREGO 8X8 COM CABECA LISO - 18,50x1,30mm DIAM</t>
+        </is>
+      </c>
+      <c r="C20" s="2" t="n">
+        <v>790240</v>
+      </c>
+      <c r="D20" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="F20" s="2" t="inlineStr">
+        <is>
+          <t>D0</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="n">
+        <v>160006001</v>
+      </c>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>PARAFUSO 3,5X12 CABECA CHATA PHS REBAIXADO BI</t>
+        </is>
+      </c>
+      <c r="C21" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="D21" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E21" s="2" t="inlineStr">
+        <is>
+          <t>S3</t>
+        </is>
+      </c>
+      <c r="F21" s="2" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="n">
+        <v>160002005</v>
+      </c>
+      <c r="B22" s="4" t="inlineStr">
+        <is>
+          <t>GUIA CABO / PASSA FIO 46MM +/-0,2MM - OFF WHI</t>
+        </is>
+      </c>
+      <c r="C22" s="2" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D22" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="F22" s="2" t="inlineStr">
+        <is>
+          <t>D3</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="n">
+        <v>160002005</v>
+      </c>
+      <c r="B23" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">GUIA CABO / PASSA FIO 46MM +/-0,2MM - PRETO  </t>
+        </is>
+      </c>
+      <c r="C23" s="2" t="n">
+        <v>8000</v>
+      </c>
+      <c r="D23" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="F23" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="n">
+        <v>160006016</v>
+      </c>
+      <c r="B24" s="4" t="inlineStr">
+        <is>
+          <t>PARAFUSO 3,5X12 CABECA FLANGEADA PHS BICROMAT</t>
+        </is>
+      </c>
+      <c r="C24" s="2" t="n">
+        <v>160000</v>
+      </c>
+      <c r="D24" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="F24" s="2" t="inlineStr">
+        <is>
+          <t>E0</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="n">
+        <v>160006008</v>
+      </c>
+      <c r="B25" s="4" t="inlineStr">
+        <is>
+          <t>PARAFUSO 4,5X25 CABECA CHATA PHS BICROMATIZAD</t>
+        </is>
+      </c>
+      <c r="C25" s="2" t="n">
+        <v>20000</v>
+      </c>
+      <c r="D25" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E25" s="2" t="inlineStr">
+        <is>
+          <t>S4</t>
+        </is>
+      </c>
+      <c r="F25" s="2" t="inlineStr">
+        <is>
+          <t>D0</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="n">
         <v>160006010</v>
       </c>
-      <c r="B7" s="4" t="inlineStr">
-        <is>
-          <t>PARAFUSO 4,5X50 CABECA CHATA PHS BICROMA</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>40000</v>
-      </c>
-      <c r="D7" s="2" t="inlineStr">
-        <is>
-          <t>R3E</t>
-        </is>
-      </c>
-      <c r="E7" s="2" t="inlineStr">
+      <c r="B26" s="4" t="inlineStr">
+        <is>
+          <t>PARAFUSO 4,5X50 CABECA CHATA PHS BICROMATIZAD</t>
+        </is>
+      </c>
+      <c r="C26" s="2" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D26" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
         <is>
           <t>S5</t>
         </is>
       </c>
-      <c r="F7" s="2" t="inlineStr">
+      <c r="F26" s="2" t="inlineStr">
+        <is>
+          <t>D0</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="n">
+        <v>160006006</v>
+      </c>
+      <c r="B27" s="4" t="inlineStr">
+        <is>
+          <t>PARAFUSO 3,5X40 CABECA CHATA PHS BICROMATIZAD</t>
+        </is>
+      </c>
+      <c r="C27" s="2" t="n">
+        <v>35000</v>
+      </c>
+      <c r="D27" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E27" s="2" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="F27" s="2" t="inlineStr">
+        <is>
+          <t>E0</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="n">
+        <v>160006022</v>
+      </c>
+      <c r="B28" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PARAFUSO M4 12MM CHATA PHS BICROMATIZADO     </t>
+        </is>
+      </c>
+      <c r="C28" s="2" t="n">
+        <v>3000</v>
+      </c>
+      <c r="D28" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E28" s="2" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="F28" s="2" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="n">
+        <v>160006042</v>
+      </c>
+      <c r="B29" s="4" t="inlineStr">
+        <is>
+          <t>PARAFUSO 3,5X30 CABECA FLANGEADA BICROMATIZAD</t>
+        </is>
+      </c>
+      <c r="C29" s="2" t="n">
+        <v>16000</v>
+      </c>
+      <c r="D29" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
+        <is>
+          <t>S5</t>
+        </is>
+      </c>
+      <c r="F29" s="2" t="inlineStr">
+        <is>
+          <t>E3</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="n">
+        <v>160001050</v>
+      </c>
+      <c r="B30" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FITA DUPLA FACE VHB 4312 25X19MM             </t>
+        </is>
+      </c>
+      <c r="C30" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="D30" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
+        <is>
+          <t>S6</t>
+        </is>
+      </c>
+      <c r="F30" s="2" t="inlineStr">
+        <is>
+          <t>E1</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="n">
+        <v>160004001</v>
+      </c>
+      <c r="B31" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUPORTE PRATELEIRA U SEM PINO CROMADO  PARA </t>
+        </is>
+      </c>
+      <c r="C31" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D31" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>S7</t>
+        </is>
+      </c>
+      <c r="F31" s="2" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="n">
+        <v>160001034</v>
+      </c>
+      <c r="B32" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CHAPA JUNCAO 18X40 COM 2 FUROS               </t>
+        </is>
+      </c>
+      <c r="C32" s="2" t="n">
+        <v>12000</v>
+      </c>
+      <c r="D32" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
+        <is>
+          <t>S7</t>
+        </is>
+      </c>
+      <c r="F32" s="2" t="inlineStr">
+        <is>
+          <t>E0</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="n">
+        <v>160001061</v>
+      </c>
+      <c r="B33" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUPORTE ANGULAR CENTRAL NATURE               </t>
+        </is>
+      </c>
+      <c r="C33" s="2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D33" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E33" s="2" t="inlineStr">
+        <is>
+          <t>S7</t>
+        </is>
+      </c>
+      <c r="F33" s="2" t="inlineStr">
+        <is>
+          <t>E2</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="n">
+        <v>160001011</v>
+      </c>
+      <c r="B34" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">SUPORTE ANGULAR CENTRAL MARRON               </t>
+        </is>
+      </c>
+      <c r="C34" s="2" t="n">
+        <v>30000</v>
+      </c>
+      <c r="D34" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E34" s="2" t="inlineStr">
+        <is>
+          <t>S8</t>
+        </is>
+      </c>
+      <c r="F34" s="2" t="inlineStr">
+        <is>
+          <t>D2</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="n">
+        <v>160001024</v>
+      </c>
+      <c r="B35" s="4" t="inlineStr">
+        <is>
+          <t>PINO GIROFIX COM ROSCA SOBERBA CONE 7MM - ACO</t>
+        </is>
+      </c>
+      <c r="C35" s="2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D35" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
+        <is>
+          <t>S8</t>
+        </is>
+      </c>
+      <c r="F35" s="2" t="inlineStr">
+        <is>
+          <t>E0</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="n">
+        <v>160001004</v>
+      </c>
+      <c r="B36" s="4" t="inlineStr">
+        <is>
+          <t xml:space="preserve">CAVILHAS 8X30MM PINUS                        </t>
+        </is>
+      </c>
+      <c r="C36" s="2" t="n">
+        <v>25000</v>
+      </c>
+      <c r="D36" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
+        <is>
+          <t>S9</t>
+        </is>
+      </c>
+      <c r="F36" s="2" t="inlineStr">
+        <is>
+          <t>D1</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="n">
+        <v>160001025</v>
+      </c>
+      <c r="B37" s="4" t="inlineStr">
+        <is>
+          <t>CASTANHA DO MINI-GIROFIX 12X9MM  **MODELO NOV</t>
+        </is>
+      </c>
+      <c r="C37" s="2" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D37" s="2" t="inlineStr">
+        <is>
+          <t>R3E</t>
+        </is>
+      </c>
+      <c r="E37" s="2" t="inlineStr">
+        <is>
+          <t>S9</t>
+        </is>
+      </c>
+      <c r="F37" s="2" t="inlineStr">
         <is>
           <t>D0</t>
         </is>

</xml_diff>